<commit_message>
Cập nhật ngày 3-5-2018
- Thêm chức năng Đăng tin
- Thêm chức năng Xem chi tiết sản phẩm
</commit_message>
<xml_diff>
--- a/web nguoi yeu cu.xlsx
+++ b/web nguoi yeu cu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Nhiệm vụ" sheetId="48" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="362">
   <si>
     <t>Tên chức năng</t>
   </si>
@@ -1221,6 +1221,15 @@
   </si>
   <si>
     <t>Viết code logic</t>
+  </si>
+  <si>
+    <t>Thông báo mặt hàng đã bán hết</t>
+  </si>
+  <si>
+    <t>Duyệt sản phẩm (cho phép sản phẩm được bán)</t>
+  </si>
+  <si>
+    <t>Vĩ</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1308,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1405,12 +1414,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1456,6 +1474,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1465,6 +1502,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1472,24 +1518,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1504,10 +1532,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1516,17 +1553,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1954,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1990,13 +2016,13 @@
       <c r="B2" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="27" t="s">
         <v>355</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="28">
         <v>0.5</v>
       </c>
     </row>
@@ -2007,13 +2033,13 @@
       <c r="B3" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="27" t="s">
         <v>355</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E3" s="48">
+      <c r="E3" s="28">
         <v>0.8</v>
       </c>
     </row>
@@ -2030,7 +2056,7 @@
       <c r="D4" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="28">
         <v>0.8</v>
       </c>
     </row>
@@ -2047,7 +2073,7 @@
       <c r="D5" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="28">
         <v>0.9</v>
       </c>
     </row>
@@ -2064,7 +2090,7 @@
       <c r="D6" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="28">
         <v>0.22</v>
       </c>
     </row>
@@ -2081,7 +2107,7 @@
       <c r="D7" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="28">
         <v>0.13600000000000001</v>
       </c>
     </row>
@@ -2100,27 +2126,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="25.42578125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="26" style="44" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="25.42578125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="59.5703125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="26" style="24" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2212,17 +2238,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>288</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2281,7 +2307,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="25" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2316,27 +2342,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="34.140625" style="44" customWidth="1"/>
-    <col min="3" max="3" width="39" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="44" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="34.140625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="39" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>297</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2420,27 +2446,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="22.28515625" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5703125" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.42578125" style="44" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="22.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.42578125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2532,17 +2558,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2564,7 +2590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="44" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="24" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -2582,7 +2608,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="44" customFormat="1" ht="86.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="24" customFormat="1" ht="86.25" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2600,11 +2626,11 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="44" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" s="44" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" s="44" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:9" s="44" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:9" s="44" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" s="24" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C9" s="12" t="s">
         <v>254</v>
       </c>
@@ -2630,27 +2656,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="27.5703125" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" style="44" customWidth="1"/>
-    <col min="4" max="4" width="48.5703125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="44" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="27.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="24" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2709,7 +2735,7 @@
       <c r="F4" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="26" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2744,27 +2770,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="32.140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="46.85546875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="44" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="32.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="24" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>326</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2817,7 +2843,7 @@
       <c r="F4" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="25" t="s">
         <v>295</v>
       </c>
     </row>
@@ -2860,17 +2886,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>335</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2950,27 +2976,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="44"/>
-    <col min="2" max="2" width="28" style="44" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" style="44" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="44" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="44" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="44"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="28" style="24" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="24" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>336</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3062,17 +3088,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>341</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -3406,11 +3432,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,7 +3448,7 @@
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3432,14 +3458,14 @@
       <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="29" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3449,14 +3475,14 @@
       <c r="C2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="30" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3466,14 +3492,14 @@
       <c r="C3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="30" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3483,14 +3509,14 @@
       <c r="C4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D4" s="30" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3500,12 +3526,12 @@
       <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3515,12 +3541,12 @@
       <c r="C6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="30" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3530,12 +3556,17 @@
       <c r="C7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3545,12 +3576,20 @@
       <c r="C8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" t="s">
+        <v>361</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3560,12 +3599,12 @@
       <c r="C9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3575,12 +3614,12 @@
       <c r="C10" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3590,12 +3629,12 @@
       <c r="C11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="50" t="s">
-        <v>13</v>
+      <c r="D11" s="30" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3605,12 +3644,17 @@
       <c r="C12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3620,12 +3664,17 @@
       <c r="C13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3635,12 +3684,12 @@
       <c r="C14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3650,12 +3699,12 @@
       <c r="C15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3665,7 +3714,7 @@
       <c r="C16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="3"/>
@@ -3680,7 +3729,7 @@
       <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="3"/>
@@ -3695,7 +3744,7 @@
       <c r="C18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="3"/>
@@ -3710,7 +3759,7 @@
       <c r="C19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="51" t="s">
+      <c r="D19" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="3"/>
@@ -3725,7 +3774,7 @@
       <c r="C20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="51" t="s">
+      <c r="D20" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="3"/>
@@ -3740,7 +3789,7 @@
       <c r="C21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="51" t="s">
+      <c r="D21" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E21" s="3"/>
@@ -3755,7 +3804,7 @@
       <c r="C22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="51" t="s">
+      <c r="D22" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="3"/>
@@ -3770,15 +3819,39 @@
       <c r="C23" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E24" s="3">
-        <f>COUNTIF(E2:E23, "Hoàn thành")/COUNTA(A2:A23)</f>
-        <v>0.13636363636363635</v>
+      <c r="B24" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="3">
+        <f>COUNTIF(E2:E25, "Hoàn thành")/COUNTA(A2:A25)</f>
+        <v>0.36363636363636365</v>
       </c>
     </row>
   </sheetData>
@@ -3808,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K92"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3830,30 +3903,30 @@
     <row r="2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="34" t="s">
+      <c r="C23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="33"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="2" t="s">
         <v>118</v>
       </c>
@@ -3880,13 +3953,13 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="41">
         <v>1</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="36" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -3909,9 +3982,9 @@
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="24"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="3" t="s">
         <v>86</v>
       </c>
@@ -3930,9 +4003,9 @@
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="24"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="3" t="s">
         <v>87</v>
       </c>
@@ -3949,9 +4022,9 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="24"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="3" t="s">
         <v>88</v>
       </c>
@@ -3968,9 +4041,9 @@
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="24"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="37"/>
       <c r="D29" s="3" t="s">
         <v>89</v>
       </c>
@@ -3987,9 +4060,9 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="24"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="3" t="s">
         <v>90</v>
       </c>
@@ -4006,9 +4079,9 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="24"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="37"/>
       <c r="D31" s="3" t="s">
         <v>91</v>
       </c>
@@ -4027,9 +4100,9 @@
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="24"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="37"/>
       <c r="D32" s="3" t="s">
         <v>92</v>
       </c>
@@ -4046,9 +4119,9 @@
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="24"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="3" t="s">
         <v>93</v>
       </c>
@@ -4067,9 +4140,9 @@
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="25"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="3" t="s">
         <v>94</v>
       </c>
@@ -4088,13 +4161,13 @@
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
+      <c r="A35" s="41">
         <v>2</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="42" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="36" t="s">
         <v>123</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -4117,9 +4190,9 @@
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="24"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="37"/>
       <c r="D36" s="3" t="s">
         <v>85</v>
       </c>
@@ -4140,9 +4213,9 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="27"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="3" t="s">
         <v>159</v>
       </c>
@@ -4163,9 +4236,9 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="24"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="37"/>
       <c r="D38" s="3" t="s">
         <v>125</v>
       </c>
@@ -4182,9 +4255,9 @@
       <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="3" t="s">
         <v>126</v>
       </c>
@@ -4201,9 +4274,9 @@
       <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="24"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="3" t="s">
         <v>127</v>
       </c>
@@ -4220,9 +4293,9 @@
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="24"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="3" t="s">
         <v>128</v>
       </c>
@@ -4239,9 +4312,9 @@
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="38"/>
       <c r="D42" s="3" t="s">
         <v>129</v>
       </c>
@@ -4260,13 +4333,13 @@
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="29">
+      <c r="A43" s="41">
         <v>3</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="45" t="s">
         <v>144</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -4287,9 +4360,9 @@
       <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="3" t="s">
         <v>145</v>
       </c>
@@ -4306,13 +4379,13 @@
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
+      <c r="A45" s="41">
         <v>4</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="42" t="s">
         <v>148</v>
       </c>
       <c r="D45" s="11" t="s">
@@ -4335,9 +4408,9 @@
       <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
       <c r="D46" s="11" t="s">
         <v>151</v>
       </c>
@@ -4354,9 +4427,9 @@
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="28"/>
-      <c r="C47" s="28"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="11" t="s">
         <v>153</v>
       </c>
@@ -4375,13 +4448,13 @@
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29">
+      <c r="A48" s="41">
         <v>5</v>
       </c>
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="36" t="s">
+      <c r="C48" s="46" t="s">
         <v>158</v>
       </c>
       <c r="D48" s="11" t="s">
@@ -4404,9 +4477,9 @@
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="37"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="47"/>
       <c r="D49" s="11" t="s">
         <v>130</v>
       </c>
@@ -4427,9 +4500,9 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
-      <c r="B50" s="28"/>
-      <c r="C50" s="38"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="48"/>
       <c r="D50" s="11" t="s">
         <v>161</v>
       </c>
@@ -4446,13 +4519,13 @@
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="29">
+      <c r="A51" s="41">
         <v>6</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="41" t="s">
         <v>164</v>
       </c>
       <c r="D51" s="11" t="s">
@@ -4477,9 +4550,9 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="26"/>
+      <c r="A52" s="41"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="18" t="s">
         <v>149</v>
       </c>
@@ -4502,13 +4575,13 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="26">
+      <c r="A53" s="42">
         <v>7</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="36" t="s">
         <v>168</v>
       </c>
       <c r="D53" s="11" t="s">
@@ -4531,9 +4604,9 @@
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="24"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="37"/>
       <c r="D54" s="11" t="s">
         <v>124</v>
       </c>
@@ -4554,9 +4627,9 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="24"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="37"/>
       <c r="D55" s="11" t="s">
         <v>171</v>
       </c>
@@ -4573,9 +4646,9 @@
       <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="25"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="38"/>
       <c r="D56" s="11" t="s">
         <v>230</v>
       </c>
@@ -4594,13 +4667,13 @@
       <c r="K56" s="3"/>
     </row>
     <row r="57" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="39">
+      <c r="A57" s="40">
         <v>8</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C57" s="40" t="s">
         <v>175</v>
       </c>
       <c r="D57" s="11" t="s">
@@ -4625,9 +4698,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="39"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="39"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="11" t="s">
         <v>124</v>
       </c>
@@ -4650,13 +4723,13 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="23">
+      <c r="A59" s="36">
         <v>9</v>
       </c>
-      <c r="B59" s="26" t="s">
+      <c r="B59" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="C59" s="23" t="s">
+      <c r="C59" s="36" t="s">
         <v>237</v>
       </c>
       <c r="D59" s="11" t="s">
@@ -4677,9 +4750,9 @@
       <c r="K59" s="3"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="24"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="37"/>
       <c r="D60" s="11" t="s">
         <v>241</v>
       </c>
@@ -4696,9 +4769,9 @@
       <c r="K60" s="3"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="25"/>
+      <c r="A61" s="38"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="38"/>
       <c r="D61" s="11" t="s">
         <v>124</v>
       </c>
@@ -4719,19 +4792,19 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="40" t="s">
+      <c r="A63" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
@@ -4749,7 +4822,7 @@
       <c r="C66" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E66" s="24" t="s">
+      <c r="E66" s="37" t="s">
         <v>198</v>
       </c>
       <c r="F66" s="21" t="s">
@@ -4760,7 +4833,7 @@
       <c r="C67" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E67" s="24"/>
+      <c r="E67" s="37"/>
       <c r="F67" s="3" t="s">
         <v>205</v>
       </c>
@@ -4769,7 +4842,7 @@
       <c r="C68" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="E68" s="24"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="3" t="s">
         <v>206</v>
       </c>
@@ -4778,7 +4851,7 @@
       <c r="C69" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E69" s="24"/>
+      <c r="E69" s="37"/>
       <c r="F69" s="3" t="s">
         <v>207</v>
       </c>
@@ -4787,7 +4860,7 @@
       <c r="C70" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E70" s="24"/>
+      <c r="E70" s="37"/>
       <c r="F70" s="3" t="s">
         <v>208</v>
       </c>
@@ -4796,7 +4869,7 @@
       <c r="C71" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E71" s="24"/>
+      <c r="E71" s="37"/>
       <c r="F71" s="3" t="s">
         <v>209</v>
       </c>
@@ -4805,7 +4878,7 @@
       <c r="C72" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="E72" s="25"/>
+      <c r="E72" s="38"/>
       <c r="F72" s="3" t="s">
         <v>210</v>
       </c>
@@ -4814,7 +4887,7 @@
       <c r="C73" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="E73" s="23" t="s">
+      <c r="E73" s="36" t="s">
         <v>199</v>
       </c>
       <c r="F73" s="3" t="s">
@@ -4825,7 +4898,7 @@
       <c r="C74" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="E74" s="24"/>
+      <c r="E74" s="37"/>
       <c r="F74" s="3" t="s">
         <v>212</v>
       </c>
@@ -4834,7 +4907,7 @@
       <c r="C75" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="E75" s="24"/>
+      <c r="E75" s="37"/>
       <c r="F75" s="3" t="s">
         <v>213</v>
       </c>
@@ -4843,7 +4916,7 @@
       <c r="C76" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E76" s="24"/>
+      <c r="E76" s="37"/>
       <c r="F76" s="3" t="s">
         <v>214</v>
       </c>
@@ -4852,7 +4925,7 @@
       <c r="C77" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E77" s="25"/>
+      <c r="E77" s="38"/>
       <c r="F77" s="3" t="s">
         <v>215</v>
       </c>
@@ -4861,7 +4934,7 @@
       <c r="C78" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E78" s="23" t="s">
+      <c r="E78" s="36" t="s">
         <v>200</v>
       </c>
       <c r="F78" s="3" t="s">
@@ -4872,7 +4945,7 @@
       <c r="C79" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E79" s="24"/>
+      <c r="E79" s="37"/>
       <c r="F79" s="3" t="s">
         <v>217</v>
       </c>
@@ -4881,7 +4954,7 @@
       <c r="C80" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="E80" s="24"/>
+      <c r="E80" s="37"/>
       <c r="F80" s="3" t="s">
         <v>218</v>
       </c>
@@ -4890,7 +4963,7 @@
       <c r="C81" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="E81" s="25"/>
+      <c r="E81" s="38"/>
       <c r="F81" s="3" t="s">
         <v>219</v>
       </c>
@@ -4899,7 +4972,7 @@
       <c r="C82" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="E82" s="23" t="s">
+      <c r="E82" s="36" t="s">
         <v>201</v>
       </c>
       <c r="F82" s="3" t="s">
@@ -4910,7 +4983,7 @@
       <c r="C83" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E83" s="24"/>
+      <c r="E83" s="37"/>
       <c r="F83" s="3" t="s">
         <v>221</v>
       </c>
@@ -4919,7 +4992,7 @@
       <c r="C84" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E84" s="24"/>
+      <c r="E84" s="37"/>
       <c r="F84" s="3" t="s">
         <v>222</v>
       </c>
@@ -4928,7 +5001,7 @@
       <c r="C85" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E85" s="24"/>
+      <c r="E85" s="37"/>
       <c r="F85" s="3" t="s">
         <v>223</v>
       </c>
@@ -4937,19 +5010,19 @@
       <c r="C86" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="E86" s="24"/>
+      <c r="E86" s="37"/>
       <c r="F86" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E87" s="25"/>
+      <c r="E87" s="38"/>
       <c r="F87" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E88" s="39" t="s">
+      <c r="E88" s="40" t="s">
         <v>226</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -4957,46 +5030,46 @@
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E89" s="39"/>
+      <c r="E89" s="40"/>
       <c r="F89" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E90" s="39"/>
+      <c r="E90" s="40"/>
       <c r="F90" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E91" s="39"/>
+      <c r="E91" s="40"/>
       <c r="F91" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E92" s="39"/>
+      <c r="E92" s="40"/>
       <c r="F92" s="11" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A63:K63"/>
-    <mergeCell ref="E66:E72"/>
-    <mergeCell ref="E73:E77"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="E82:E87"/>
-    <mergeCell ref="E88:E92"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:K23"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C25:C34"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="A51:A52"/>
@@ -5004,21 +5077,21 @@
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="C45:C47"/>
     <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D23:K23"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C25:C34"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C35:C42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="E82:E87"/>
+    <mergeCell ref="E88:E92"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="E66:E72"/>
+    <mergeCell ref="E73:E77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5046,17 +5119,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5115,33 +5188,33 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C9" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="55" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="55"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -5224,17 +5297,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5326,17 +5399,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>255</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5354,7 +5427,7 @@
       <c r="E2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="23" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5410,17 +5483,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -5497,7 +5570,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5510,17 +5583,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="54" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
     </row>
     <row r="2" spans="1:9" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">

</xml_diff>

<commit_message>
thêm Hiển thị danh sách sản phẩm theo loại
</commit_message>
<xml_diff>
--- a/web nguoi yeu cu.xlsx
+++ b/web nguoi yeu cu.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="362">
   <si>
     <t>Tên chức năng</t>
   </si>
@@ -1227,6 +1227,9 @@
   </si>
   <si>
     <t>Duyệt sản phẩm (cho phép sản phẩm được bán)</t>
+  </si>
+  <si>
+    <t>Vĩ</t>
   </si>
 </sst>
 </file>
@@ -1499,6 +1502,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1506,24 +1518,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1538,10 +1532,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3429,11 +3432,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3448,7 @@
     <col min="5" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3496,7 +3499,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3513,7 +3516,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3528,7 +3531,7 @@
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3543,7 +3546,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3559,8 +3562,11 @@
       <c r="E7" s="3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3576,8 +3582,14 @@
       <c r="E8" s="3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>361</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3592,7 +3604,7 @@
       </c>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3607,7 +3619,7 @@
       </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3622,7 +3634,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3638,8 +3650,11 @@
       <c r="E12" s="3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3655,8 +3670,11 @@
       <c r="E13" s="3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3671,7 +3689,7 @@
       </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3686,7 +3704,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3885,30 +3903,30 @@
     <row r="2" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="D23" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="43"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+      <c r="A24" s="53"/>
+      <c r="B24" s="52"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="2" t="s">
         <v>118</v>
       </c>
@@ -3935,10 +3953,10 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="42">
+      <c r="A25" s="41">
         <v>1</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="36" t="s">
@@ -3964,8 +3982,8 @@
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="40"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="43"/>
       <c r="C26" s="37"/>
       <c r="D26" s="3" t="s">
         <v>86</v>
@@ -3985,8 +4003,8 @@
       <c r="K26" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="40"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="43"/>
       <c r="C27" s="37"/>
       <c r="D27" s="3" t="s">
         <v>87</v>
@@ -4004,8 +4022,8 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="40"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="37"/>
       <c r="D28" s="3" t="s">
         <v>88</v>
@@ -4023,8 +4041,8 @@
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="37"/>
       <c r="D29" s="3" t="s">
         <v>89</v>
@@ -4042,8 +4060,8 @@
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="43"/>
       <c r="C30" s="37"/>
       <c r="D30" s="3" t="s">
         <v>90</v>
@@ -4061,8 +4079,8 @@
       <c r="K30" s="3"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="43"/>
       <c r="C31" s="37"/>
       <c r="D31" s="3" t="s">
         <v>91</v>
@@ -4082,8 +4100,8 @@
       <c r="K31" s="3"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="42"/>
-      <c r="B32" s="40"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="43"/>
       <c r="C32" s="37"/>
       <c r="D32" s="3" t="s">
         <v>92</v>
@@ -4101,8 +4119,8 @@
       <c r="K32" s="3"/>
     </row>
     <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="42"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="37"/>
       <c r="D33" s="3" t="s">
         <v>93</v>
@@ -4122,8 +4140,8 @@
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="41"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="38"/>
       <c r="D34" s="3" t="s">
         <v>94</v>
@@ -4143,10 +4161,10 @@
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="42">
+      <c r="A35" s="41">
         <v>2</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B35" s="42" t="s">
         <v>122</v>
       </c>
       <c r="C35" s="36" t="s">
@@ -4172,8 +4190,8 @@
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="40"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="37"/>
       <c r="D36" s="3" t="s">
         <v>85</v>
@@ -4195,8 +4213,8 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="37"/>
       <c r="D37" s="3" t="s">
         <v>159</v>
@@ -4218,8 +4236,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="43"/>
       <c r="C38" s="37"/>
       <c r="D38" s="3" t="s">
         <v>125</v>
@@ -4237,8 +4255,8 @@
       <c r="K38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="43"/>
       <c r="C39" s="37"/>
       <c r="D39" s="3" t="s">
         <v>126</v>
@@ -4256,8 +4274,8 @@
       <c r="K39" s="3"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
-      <c r="B40" s="40"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="43"/>
       <c r="C40" s="37"/>
       <c r="D40" s="3" t="s">
         <v>127</v>
@@ -4275,8 +4293,8 @@
       <c r="K40" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
-      <c r="B41" s="40"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="43"/>
       <c r="C41" s="37"/>
       <c r="D41" s="3" t="s">
         <v>128</v>
@@ -4294,8 +4312,8 @@
       <c r="K41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="41"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="44"/>
       <c r="C42" s="38"/>
       <c r="D42" s="3" t="s">
         <v>129</v>
@@ -4315,13 +4333,13 @@
       <c r="K42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="42">
+      <c r="A43" s="41">
         <v>3</v>
       </c>
-      <c r="B43" s="48" t="s">
+      <c r="B43" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="C43" s="48" t="s">
+      <c r="C43" s="45" t="s">
         <v>144</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -4342,9 +4360,9 @@
       <c r="K43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="48"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
       <c r="D44" s="3" t="s">
         <v>145</v>
       </c>
@@ -4361,13 +4379,13 @@
       <c r="K44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="42">
+      <c r="A45" s="41">
         <v>4</v>
       </c>
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="42" t="s">
         <v>148</v>
       </c>
       <c r="D45" s="11" t="s">
@@ -4390,9 +4408,9 @@
       <c r="K45" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
       <c r="D46" s="11" t="s">
         <v>151</v>
       </c>
@@ -4409,9 +4427,9 @@
       <c r="K46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="11" t="s">
         <v>153</v>
       </c>
@@ -4430,13 +4448,13 @@
       <c r="K47" s="3"/>
     </row>
     <row r="48" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="42">
+      <c r="A48" s="41">
         <v>5</v>
       </c>
-      <c r="B48" s="39" t="s">
+      <c r="B48" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="49" t="s">
+      <c r="C48" s="46" t="s">
         <v>158</v>
       </c>
       <c r="D48" s="11" t="s">
@@ -4459,9 +4477,9 @@
       <c r="K48" s="3"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="50"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="47"/>
       <c r="D49" s="11" t="s">
         <v>130</v>
       </c>
@@ -4482,9 +4500,9 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="51"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="48"/>
       <c r="D50" s="11" t="s">
         <v>161</v>
       </c>
@@ -4501,13 +4519,13 @@
       <c r="K50" s="3"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="42">
+      <c r="A51" s="41">
         <v>6</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="41" t="s">
         <v>164</v>
       </c>
       <c r="D51" s="11" t="s">
@@ -4532,9 +4550,9 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="42"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="39"/>
+      <c r="A52" s="41"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="18" t="s">
         <v>149</v>
       </c>
@@ -4557,10 +4575,10 @@
       </c>
     </row>
     <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39">
+      <c r="A53" s="42">
         <v>7</v>
       </c>
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="42" t="s">
         <v>167</v>
       </c>
       <c r="C53" s="36" t="s">
@@ -4586,8 +4604,8 @@
       <c r="K53" s="3"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
-      <c r="B54" s="40"/>
+      <c r="A54" s="43"/>
+      <c r="B54" s="43"/>
       <c r="C54" s="37"/>
       <c r="D54" s="11" t="s">
         <v>124</v>
@@ -4609,8 +4627,8 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
-      <c r="B55" s="40"/>
+      <c r="A55" s="43"/>
+      <c r="B55" s="43"/>
       <c r="C55" s="37"/>
       <c r="D55" s="11" t="s">
         <v>171</v>
@@ -4628,8 +4646,8 @@
       <c r="K55" s="3"/>
     </row>
     <row r="56" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
-      <c r="B56" s="41"/>
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
       <c r="C56" s="38"/>
       <c r="D56" s="11" t="s">
         <v>230</v>
@@ -4649,13 +4667,13 @@
       <c r="K56" s="3"/>
     </row>
     <row r="57" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="52">
+      <c r="A57" s="40">
         <v>8</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="40" t="s">
         <v>175</v>
       </c>
       <c r="D57" s="11" t="s">
@@ -4680,9 +4698,9 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="52"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="40"/>
       <c r="D58" s="11" t="s">
         <v>124</v>
       </c>
@@ -4708,7 +4726,7 @@
       <c r="A59" s="36">
         <v>9</v>
       </c>
-      <c r="B59" s="39" t="s">
+      <c r="B59" s="42" t="s">
         <v>236</v>
       </c>
       <c r="C59" s="36" t="s">
@@ -4733,7 +4751,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="37"/>
-      <c r="B60" s="40"/>
+      <c r="B60" s="43"/>
       <c r="C60" s="37"/>
       <c r="D60" s="11" t="s">
         <v>241</v>
@@ -4752,7 +4770,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="38"/>
-      <c r="B61" s="41"/>
+      <c r="B61" s="44"/>
       <c r="C61" s="38"/>
       <c r="D61" s="11" t="s">
         <v>124</v>
@@ -4774,19 +4792,19 @@
       </c>
     </row>
     <row r="63" spans="1:11" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="53" t="s">
+      <c r="A63" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="B63" s="53"/>
-      <c r="C63" s="53"/>
-      <c r="D63" s="53"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53"/>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53"/>
-      <c r="K63" s="53"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="39"/>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
@@ -5004,7 +5022,7 @@
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E88" s="52" t="s">
+      <c r="E88" s="40" t="s">
         <v>226</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -5012,46 +5030,46 @@
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E89" s="52"/>
+      <c r="E89" s="40"/>
       <c r="F89" s="3" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E90" s="52"/>
+      <c r="E90" s="40"/>
       <c r="F90" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E91" s="52"/>
+      <c r="E91" s="40"/>
       <c r="F91" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="E92" s="52"/>
+      <c r="E92" s="40"/>
       <c r="F92" s="11" t="s">
         <v>202</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="A63:K63"/>
-    <mergeCell ref="E66:E72"/>
-    <mergeCell ref="E73:E77"/>
-    <mergeCell ref="E78:E81"/>
-    <mergeCell ref="E82:E87"/>
-    <mergeCell ref="E88:E92"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="C35:C42"/>
+    <mergeCell ref="B35:B42"/>
+    <mergeCell ref="A35:A42"/>
+    <mergeCell ref="A25:A34"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="D23:K23"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C25:C34"/>
+    <mergeCell ref="B25:B34"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="A51:A52"/>
@@ -5059,21 +5077,21 @@
     <mergeCell ref="B45:B47"/>
     <mergeCell ref="C45:C47"/>
     <mergeCell ref="A45:A47"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="D23:K23"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C25:C34"/>
-    <mergeCell ref="B25:B34"/>
-    <mergeCell ref="C35:C42"/>
-    <mergeCell ref="B35:B42"/>
-    <mergeCell ref="A35:A42"/>
-    <mergeCell ref="A25:A34"/>
-    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="C53:C56"/>
+    <mergeCell ref="E78:E81"/>
+    <mergeCell ref="E82:E87"/>
+    <mergeCell ref="E88:E92"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="C59:C61"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="E66:E72"/>
+    <mergeCell ref="E73:E77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>